<commit_message>
Control de errores y corrección en monto
Se estaba agregando consistentemente un cero de más al final del monto. Además se modifica el control de errores para informar en caso de fallas en archivos específicos, sin que esto impida la ejecución del resto del parser.
</commit_message>
<xml_diff>
--- a/Nevasa/CompraSimultanea/20240826/20240826_nevasa_compras_simultaneas_results.xlsx
+++ b/Nevasa/CompraSimultanea/20240826/20240826_nevasa_compras_simultaneas_results.xlsx
@@ -479,7 +479,7 @@
         <v>35802360</v>
       </c>
       <c r="C2" t="n">
-        <v>360518400</v>
+        <v>36051840</v>
       </c>
       <c r="D2" t="n">
         <v>0.6</v>
@@ -501,7 +501,7 @@
         <v>47615040</v>
       </c>
       <c r="C3" t="n">
-        <v>478594670</v>
+        <v>47859467</v>
       </c>
       <c r="D3" t="n">
         <v>0.55</v>
@@ -523,7 +523,7 @@
         <v>18227000</v>
       </c>
       <c r="C4" t="n">
-        <v>183188640</v>
+        <v>18318864</v>
       </c>
       <c r="D4" t="n">
         <v>0.54</v>
@@ -545,7 +545,7 @@
         <v>37986000</v>
       </c>
       <c r="C5" t="n">
-        <v>385966880</v>
+        <v>38596688</v>
       </c>
       <c r="D5" t="n">
         <v>0.53</v>
@@ -567,7 +567,7 @@
         <v>32605854</v>
       </c>
       <c r="C6" t="n">
-        <v>327786700</v>
+        <v>32778670</v>
       </c>
       <c r="D6" t="n">
         <v>0.53</v>
@@ -589,7 +589,7 @@
         <v>54737607</v>
       </c>
       <c r="C7" t="n">
-        <v>550277240</v>
+        <v>55027724</v>
       </c>
       <c r="D7" t="n">
         <v>0.53</v>
@@ -611,7 +611,7 @@
         <v>14824680</v>
       </c>
       <c r="C8" t="n">
-        <v>149090760</v>
+        <v>14909076</v>
       </c>
       <c r="D8" t="n">
         <v>0.61</v>
@@ -633,7 +633,7 @@
         <v>77700000</v>
       </c>
       <c r="C9" t="n">
-        <v>794404800</v>
+        <v>79440480</v>
       </c>
       <c r="D9" t="n">
         <v>0.5600000000000001</v>
@@ -655,7 +655,7 @@
         <v>244361800</v>
       </c>
       <c r="C10" t="n">
-        <v>2456324810</v>
+        <v>245632481</v>
       </c>
       <c r="D10" t="n">
         <v>0.52</v>
@@ -677,7 +677,7 @@
         <v>27888600</v>
       </c>
       <c r="C11" t="n">
-        <v>280419870</v>
+        <v>28041987</v>
       </c>
       <c r="D11" t="n">
         <v>0.55</v>

</xml_diff>